<commit_message>
Commiting the recent changes and issues fixes in scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataSheet.xlsx
+++ b/src/test/resources/TestDataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17860" activeTab="1"/>
+    <workbookView windowHeight="16420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignInTest" sheetId="1" r:id="rId1"/>
@@ -56,16 +56,16 @@
     <t>Maiidf@iir</t>
   </si>
   <si>
-    <t>TC_008_SignUnTest</t>
+    <t>TC_008_SignUpTest</t>
   </si>
   <si>
     <t>Maginthanofficial1@gmail.com</t>
   </si>
   <si>
-    <t>TC_009_SignUnTest</t>
-  </si>
-  <si>
-    <t>TC_010_SignUnTest</t>
+    <t>TC_009_SignUpTest</t>
+  </si>
+  <si>
+    <t>TC_010_SignUpTest</t>
   </si>
 </sst>
 </file>
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -108,6 +108,44 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -119,121 +157,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,73 +248,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,109 +416,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,6 +439,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -460,43 +475,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,16 +506,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,147 +528,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1148,15 +1148,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3"/>
+    <row r="4" spans="2:2">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="Maiidf@iir"/>
+    <hyperlink ref="A2" r:id="rId1" display="Maiidf@iir" tooltip="mailto:Maiidf@iir"/>
     <hyperlink ref="A3" r:id="rId2" display="Maginthanofficial1@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>